<commit_message>
TRA2503 fixing (column headers)
</commit_message>
<xml_diff>
--- a/inst/DfT_styles.xlsx
+++ b/inst/DfT_styles.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\virago.internal.dtlr.gov.uk\u\Lon1\LSHAW\My Documents\Temp Files (email attachments)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukeS\Documents\ac-roadtraff-pipe\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -71,12 +71,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -167,6 +167,13 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -225,19 +232,23 @@
     <border>
       <left/>
       <right/>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -306,8 +317,8 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -339,7 +350,13 @@
     <xdr:ext cx="847721" cy="723903"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 5"/>
+        <xdr:cNvPr id="2" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -377,7 +394,13 @@
     <xdr:ext cx="1542857" cy="1009525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 6"/>
+        <xdr:cNvPr id="3" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -672,8 +695,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -760,7 +783,7 @@
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="16"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="17" t="s">
         <v>9</v>
       </c>
@@ -778,16 +801,16 @@
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="20"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+    <row r="26" spans="1:1" ht="59.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="22" t="s">
+    <row r="28" spans="1:1" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding dotted line to styles
</commit_message>
<xml_diff>
--- a/inst/DfT_styles.xlsx
+++ b/inst/DfT_styles.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukeS\Documents\ac-roadtraff-pipe\inst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\virago.internal.dtlr.gov.uk\ts\LON1\LSHAW\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>header</t>
   </si>
@@ -66,12 +66,15 @@
   </si>
   <si>
     <t>ch_bottom</t>
+  </si>
+  <si>
+    <t>body_topline_dashed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
@@ -192,7 +195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -253,12 +256,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -319,6 +331,9 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -353,7 +368,7 @@
         <xdr:cNvPr id="2" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -397,7 +412,7 @@
         <xdr:cNvPr id="3" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -695,8 +710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -814,6 +829,11 @@
         <v>13</v>
       </c>
     </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="42" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>